<commit_message>
sql : [zsp_Logging_Stat2] avg - N * stdevp maybe < 0
</commit_message>
<xml_diff>
--- a/Samples/MsSqlCodeDiffVersioning/MsSqlCodeDiffVersioning.Shared/00.PerfTest/10.Results/PerfTest.Web.IO.xlsx
+++ b/Samples/MsSqlCodeDiffVersioning/MsSqlCodeDiffVersioning.Shared/00.PerfTest/10.Results/PerfTest.Web.IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGitHub\Microshaoft.Common.Utilities.Net\Samples\MsSqlCodeDiffVersioning\MsSqlCodeDiffVersioning.Shared\00.PerfTest\10.Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829B72C2-7204-4D92-BD50-07F1F2AF99BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F03EEEA-DF50-4A01-82D4-1B4D6B759F0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{AE915694-6CCA-43E3-8E29-7965574BE3FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>WINDOWS</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>2020-02-03 01:49:58.000</t>
+  </si>
+  <si>
+    <t>2020-02-03 02:26:09.000</t>
+  </si>
+  <si>
+    <t>2020-02-03 02:26:31.000</t>
+  </si>
+  <si>
+    <t>2020-02-03 02:30:01.000</t>
   </si>
 </sst>
 </file>
@@ -196,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +217,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -294,6 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,13 +927,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CDA3A2-7FAE-4DCA-B4B0-FAB3062786AF}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1242,63 +1259,63 @@
         <v>39</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="13">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="F6" s="13">
-        <v>22.287500000000001</v>
+        <v>11.3048</v>
       </c>
       <c r="G6" s="13">
-        <v>38.448881</v>
+        <v>27.370142999999999</v>
       </c>
       <c r="H6" s="13">
-        <v>215.57919999999999</v>
+        <v>788.68650000000002</v>
       </c>
       <c r="I6" s="13">
-        <v>44.334000000000003</v>
+        <v>14.844799999999999</v>
       </c>
       <c r="J6" s="13">
-        <v>12.4006436410259</v>
+        <v>17.833967568693101</v>
       </c>
       <c r="K6" s="13">
         <v>10000</v>
       </c>
       <c r="L6" s="13">
-        <v>9793</v>
+        <v>9776</v>
       </c>
       <c r="M6" s="13">
-        <v>88.13</v>
-      </c>
-      <c r="N6" s="13">
-        <v>13.647593717948199</v>
+        <v>92.92</v>
+      </c>
+      <c r="N6" s="15">
+        <v>0</v>
       </c>
       <c r="O6" s="13">
-        <v>63.250168282051803</v>
+        <v>63.038078137386201</v>
       </c>
       <c r="P6" s="13">
-        <v>1</v>
+        <v>10001</v>
       </c>
       <c r="Q6" s="13">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>50</v>
@@ -1313,34 +1330,34 @@
         <v>196</v>
       </c>
       <c r="F7" s="13">
-        <v>8.6926000000000005</v>
+        <v>22.287500000000001</v>
       </c>
       <c r="G7" s="13">
-        <v>14.920427999999999</v>
+        <v>38.448881</v>
       </c>
       <c r="H7" s="13">
-        <v>192.11930000000001</v>
+        <v>215.57919999999999</v>
       </c>
       <c r="I7" s="13">
-        <v>24.967600000000001</v>
+        <v>44.334000000000003</v>
       </c>
       <c r="J7" s="13">
-        <v>5.09272201988641</v>
+        <v>12.4006436410259</v>
       </c>
       <c r="K7" s="13">
         <v>10000</v>
       </c>
       <c r="L7" s="13">
-        <v>9790</v>
+        <v>9793</v>
       </c>
       <c r="M7" s="13">
-        <v>92.54</v>
+        <v>88.13</v>
       </c>
       <c r="N7" s="13">
-        <v>4.7349839602271802</v>
+        <v>13.647593717948199</v>
       </c>
       <c r="O7" s="13">
-        <v>25.105872039772802</v>
+        <v>63.250168282051803</v>
       </c>
       <c r="P7" s="13">
         <v>1</v>
@@ -1352,6 +1369,124 @@
         <v>48</v>
       </c>
       <c r="S7" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="13">
+        <v>210</v>
+      </c>
+      <c r="F8" s="13">
+        <v>7.8936999999999999</v>
+      </c>
+      <c r="G8" s="13">
+        <v>16.373159999999999</v>
+      </c>
+      <c r="H8" s="13">
+        <v>450.78440000000001</v>
+      </c>
+      <c r="I8" s="13">
+        <v>11.305899999999999</v>
+      </c>
+      <c r="J8" s="13">
+        <v>9.55310322735399</v>
+      </c>
+      <c r="K8" s="13">
+        <v>10000</v>
+      </c>
+      <c r="L8" s="13">
+        <v>9752</v>
+      </c>
+      <c r="M8" s="13">
+        <v>91.38</v>
+      </c>
+      <c r="N8" s="15">
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <v>35.479366454708</v>
+      </c>
+      <c r="P8" s="13">
+        <v>10001</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>20000</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <v>196</v>
+      </c>
+      <c r="F9" s="13">
+        <v>8.6926000000000005</v>
+      </c>
+      <c r="G9" s="13">
+        <v>14.920427999999999</v>
+      </c>
+      <c r="H9" s="13">
+        <v>192.11930000000001</v>
+      </c>
+      <c r="I9" s="13">
+        <v>24.967600000000001</v>
+      </c>
+      <c r="J9" s="13">
+        <v>5.09272201988641</v>
+      </c>
+      <c r="K9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="13">
+        <v>9790</v>
+      </c>
+      <c r="M9" s="13">
+        <v>92.54</v>
+      </c>
+      <c r="N9" s="13">
+        <v>4.7349839602271802</v>
+      </c>
+      <c r="O9" s="13">
+        <v>25.105872039772802</v>
+      </c>
+      <c r="P9" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="S9" s="14" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>